<commit_message>
[BACK][STORIES] Manage count and list of stories for connected user
</commit_message>
<xml_diff>
--- a/tests/Postman/Tests Postman.xlsx
+++ b/tests/Postman/Tests Postman.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
   <si>
     <t>Main folder</t>
   </si>
@@ -195,9 +195,6 @@
     <t>http://localhost:8080/stories/user/{id}</t>
   </si>
   <si>
-    <t>http://localhost:8080/stories/pagin?page=0&amp;size=5&amp;sortProperty=id&amp;sortDirection=ASC</t>
-  </si>
-  <si>
     <t>http://localhost:8080/stories/user/{id}/pagin?page=0&amp;size=2&amp;sortProperty=id&amp;sortDirection=ASC</t>
   </si>
   <si>
@@ -205,6 +202,45 @@
   </si>
   <si>
     <t xml:space="preserve">List of all stories with pagination (2 results per page) </t>
+  </si>
+  <si>
+    <t>Stories Count all of Myself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/stories/count/myself </t>
+  </si>
+  <si>
+    <t>Count all stories of connected user</t>
+  </si>
+  <si>
+    <t>Stories List all of Myself</t>
+  </si>
+  <si>
+    <t>Stories List all of Myself pagination</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/stories/user/myself</t>
+  </si>
+  <si>
+    <t>Listing of all stories of connected user</t>
+  </si>
+  <si>
+    <t>List of all stories of the connected user</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/stories/user/myself/pagin?page=0&amp;size=2&amp;sortProperty=id&amp;sortDirection=ASC</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/stories/pagin?page=0&amp;size=2&amp;sortProperty=id&amp;sortDirection=ASC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of all stories of the connected user with pagination (2 results per page) </t>
+  </si>
+  <si>
+    <t>Requires header idConnectedUser with id of the connected User</t>
+  </si>
+  <si>
+    <t>Listing of all stories of connected user with pagination</t>
   </si>
 </sst>
 </file>
@@ -365,7 +401,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -427,6 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -960,7 +997,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -970,7 +1007,7 @@
     <col min="3" max="3" width="34.42578125" style="9" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="94.5703125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" style="9" customWidth="1"/>
     <col min="7" max="7" width="62.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="60.5703125" style="9" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" style="9" customWidth="1"/>
@@ -1150,22 +1187,24 @@
         <v>16</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>17</v>
+      <c r="E10" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="H10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1177,22 +1216,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1204,22 +1243,22 @@
         <v>16</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="20" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1231,26 +1270,26 @@
         <v>16</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="14" customFormat="1" ht="30">
+    <row r="14" spans="1:9" s="14" customFormat="1">
       <c r="A14" s="15" t="s">
         <v>15</v>
       </c>
@@ -1258,22 +1297,20 @@
         <v>16</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>29</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="G14" s="16"/>
       <c r="H14" s="15" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>14</v>
@@ -1287,20 +1324,22 @@
         <v>16</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="16"/>
+        <v>68</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="H15" s="15" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>14</v>
@@ -1314,26 +1353,28 @@
         <v>16</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="16"/>
+        <v>74</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="H16" s="15" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="14" customFormat="1">
+    <row r="17" spans="1:9" s="14" customFormat="1" ht="30">
       <c r="A17" s="15" t="s">
         <v>15</v>
       </c>
@@ -1341,57 +1382,107 @@
         <v>16</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="14" customFormat="1">
+      <c r="A18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="14" customFormat="1">
+      <c r="A19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="14" customFormat="1">
+      <c r="A20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E20" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F20" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="15" t="s">
+      <c r="G20" s="16"/>
+      <c r="H20" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I20" s="19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="14" customFormat="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" s="14" customFormat="1">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" s="14" customFormat="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:9" s="14" customFormat="1">
       <c r="A21" s="15"/>
@@ -2682,22 +2773,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E11" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
     <hyperlink ref="E8" r:id="rId3"/>
-    <hyperlink ref="E14" r:id="rId4"/>
-    <hyperlink ref="E15" r:id="rId5"/>
-    <hyperlink ref="E16" r:id="rId6"/>
-    <hyperlink ref="E17" r:id="rId7"/>
-    <hyperlink ref="E11" r:id="rId8"/>
+    <hyperlink ref="E17" r:id="rId4"/>
+    <hyperlink ref="E18" r:id="rId5"/>
+    <hyperlink ref="E19" r:id="rId6"/>
+    <hyperlink ref="E20" r:id="rId7"/>
+    <hyperlink ref="E12" r:id="rId8"/>
     <hyperlink ref="E9" r:id="rId9"/>
-    <hyperlink ref="E12" r:id="rId10"/>
-    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId10"/>
+    <hyperlink ref="E14" r:id="rId11"/>
+    <hyperlink ref="E10" r:id="rId12"/>
+    <hyperlink ref="E15" r:id="rId13"/>
+    <hyperlink ref="E16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[BACK][ENTITIES] Created entities Places + Timelapses + Types simple CRUDs
</commit_message>
<xml_diff>
--- a/tests/Postman/Tests Postman.xlsx
+++ b/tests/Postman/Tests Postman.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="147">
   <si>
     <t>Main folder</t>
   </si>
@@ -241,6 +241,222 @@
   </si>
   <si>
     <t>Listing of all stories of connected user with pagination</t>
+  </si>
+  <si>
+    <t>Places</t>
+  </si>
+  <si>
+    <t>Places Count all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/places/count </t>
+  </si>
+  <si>
+    <t>Count all places</t>
+  </si>
+  <si>
+    <t>Places List all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/places  </t>
+  </si>
+  <si>
+    <t>List of all places</t>
+  </si>
+  <si>
+    <t>Listing of all places</t>
+  </si>
+  <si>
+    <t>Place Create</t>
+  </si>
+  <si>
+    <t>Place Display</t>
+  </si>
+  <si>
+    <t>Place Delete</t>
+  </si>
+  <si>
+    <t>Place Update</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/places/add</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/places/display/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/places/delete/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/places/update/{id}</t>
+  </si>
+  <si>
+    <t>Create a place</t>
+  </si>
+  <si>
+    <t>Display a place</t>
+  </si>
+  <si>
+    <t>Delete a place</t>
+  </si>
+  <si>
+    <t>Update a place</t>
+  </si>
+  <si>
+    <t>Place created</t>
+  </si>
+  <si>
+    <t>Place displayed</t>
+  </si>
+  <si>
+    <t>Place deleted</t>
+  </si>
+  <si>
+    <t>Place updated</t>
+  </si>
+  <si>
+    <t>Timelapses</t>
+  </si>
+  <si>
+    <t>Timelapses Count all</t>
+  </si>
+  <si>
+    <t>Timelapses List all</t>
+  </si>
+  <si>
+    <t>Timelapse Create</t>
+  </si>
+  <si>
+    <t>Timelapse Display</t>
+  </si>
+  <si>
+    <t>Timelapse Delete</t>
+  </si>
+  <si>
+    <t>Timelapse Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/timelapses/count </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/timelapses/update/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/timelapses/delete/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/timelapses/display/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/timelapses/add</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/timelapses</t>
+  </si>
+  <si>
+    <t>Count all timelapses</t>
+  </si>
+  <si>
+    <t>Listing of all timelapses</t>
+  </si>
+  <si>
+    <t>Create a timelapse</t>
+  </si>
+  <si>
+    <t>Display a timelapse</t>
+  </si>
+  <si>
+    <t>Delete a timelapse</t>
+  </si>
+  <si>
+    <t>Update a timelapse</t>
+  </si>
+  <si>
+    <t>List of all timelapses</t>
+  </si>
+  <si>
+    <t>Timelapse deleted</t>
+  </si>
+  <si>
+    <t>Timelapse updated</t>
+  </si>
+  <si>
+    <t>Timelapse displayed</t>
+  </si>
+  <si>
+    <t>Timelapse created</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Types Count all</t>
+  </si>
+  <si>
+    <t>Types List all</t>
+  </si>
+  <si>
+    <t>Type Create</t>
+  </si>
+  <si>
+    <t>Type Display</t>
+  </si>
+  <si>
+    <t>Type Delete</t>
+  </si>
+  <si>
+    <t>Type Update</t>
+  </si>
+  <si>
+    <t>Type created</t>
+  </si>
+  <si>
+    <t>Type displayed</t>
+  </si>
+  <si>
+    <t>Type deleted</t>
+  </si>
+  <si>
+    <t>Type updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/types/count </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/types</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/types/add</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/types/display/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/types/delete/{id}</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/types/update/{id}</t>
+  </si>
+  <si>
+    <t>Update a type</t>
+  </si>
+  <si>
+    <t>Delete a type</t>
+  </si>
+  <si>
+    <t>Display a type</t>
+  </si>
+  <si>
+    <t>Create a type</t>
+  </si>
+  <si>
+    <t>Listing of all types</t>
+  </si>
+  <si>
+    <t>Count all types</t>
+  </si>
+  <si>
+    <t>List of all types</t>
   </si>
 </sst>
 </file>
@@ -279,7 +495,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +511,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +623,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -464,6 +686,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -996,8 +1224,8 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1115,15 +1343,15 @@
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" s="14" customFormat="1">
       <c r="A8" s="15" t="s">
@@ -1485,235 +1713,523 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="14" customFormat="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" s="14" customFormat="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="A22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="G22" s="16"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
+      <c r="H22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="1:9" s="14" customFormat="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="A23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>82</v>
+      </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
+      <c r="H23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:9" s="14" customFormat="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="A24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
+      <c r="H24" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="1:9" s="14" customFormat="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="A25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
+      <c r="H25" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:9" s="14" customFormat="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="A26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>93</v>
+      </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
+      <c r="H26" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="1:9" s="14" customFormat="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="A27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>94</v>
+      </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="15"/>
+      <c r="H27" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="1:9" s="14" customFormat="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" s="14" customFormat="1">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="A29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>112</v>
+      </c>
       <c r="G29" s="16"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
+      <c r="H29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="1:9" s="14" customFormat="1">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="A30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
+      <c r="H30" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:9" s="14" customFormat="1">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="A31" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>114</v>
+      </c>
       <c r="G31" s="16"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
+      <c r="H31" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:9" s="14" customFormat="1">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="A32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>115</v>
+      </c>
       <c r="G32" s="16"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:9" s="14" customFormat="1">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="A33" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="G33" s="16"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
+      <c r="H33" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:9" s="14" customFormat="1">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="A34" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>117</v>
+      </c>
       <c r="G34" s="16"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
+      <c r="H34" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:9" s="14" customFormat="1">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" s="14" customFormat="1">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="A36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>145</v>
+      </c>
       <c r="G36" s="16"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
+      <c r="H36" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="1:9" s="14" customFormat="1">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="A37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>144</v>
+      </c>
       <c r="G37" s="16"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
+      <c r="H37" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="1:9" s="14" customFormat="1">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="A38" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="G38" s="16"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
+      <c r="H38" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="I38" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:9" s="14" customFormat="1">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+      <c r="A39" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>142</v>
+      </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
+      <c r="H39" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="1:9" s="14" customFormat="1">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+      <c r="A40" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>141</v>
+      </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="15"/>
-      <c r="I40" s="15"/>
+      <c r="H40" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I40" s="20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="41" spans="1:9" s="14" customFormat="1">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
+      <c r="A41" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="G41" s="16"/>
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
+      <c r="H41" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="1:9" s="14" customFormat="1">
       <c r="A42" s="15"/>
@@ -2787,11 +3303,29 @@
     <hyperlink ref="E10" r:id="rId12"/>
     <hyperlink ref="E15" r:id="rId13"/>
     <hyperlink ref="E16" r:id="rId14"/>
+    <hyperlink ref="E22" r:id="rId15"/>
+    <hyperlink ref="E23" r:id="rId16"/>
+    <hyperlink ref="E24" r:id="rId17"/>
+    <hyperlink ref="E25" r:id="rId18"/>
+    <hyperlink ref="E26" r:id="rId19"/>
+    <hyperlink ref="E27" r:id="rId20"/>
+    <hyperlink ref="E29" r:id="rId21"/>
+    <hyperlink ref="E30" r:id="rId22"/>
+    <hyperlink ref="E31" r:id="rId23"/>
+    <hyperlink ref="E32" r:id="rId24"/>
+    <hyperlink ref="E33" r:id="rId25"/>
+    <hyperlink ref="E34" r:id="rId26"/>
+    <hyperlink ref="E36" r:id="rId27"/>
+    <hyperlink ref="E37" r:id="rId28"/>
+    <hyperlink ref="E38" r:id="rId29"/>
+    <hyperlink ref="E39" r:id="rId30"/>
+    <hyperlink ref="E40" r:id="rId31"/>
+    <hyperlink ref="E41" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
   <tableParts count="1">
-    <tablePart r:id="rId16"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[BACK][EVOL] Modifications of Controllers
</commit_message>
<xml_diff>
--- a/tests/Postman/Tests Postman.xlsx
+++ b/tests/Postman/Tests Postman.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="137">
   <si>
     <t>Main folder</t>
   </si>
@@ -401,6 +401,31 @@
   </si>
   <si>
     <t>DateCreation + user_id are automatically filled in the back from the service</t>
+  </si>
+  <si>
+    <t>Stories Count all by Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/stories/count/screen?longitudeSW=45.78&amp;latitudeSW=4.8&amp;longitudeNE=45.8&amp;latitudeNE=5 </t>
+  </si>
+  <si>
+    <t>Count all stories within the screen</t>
+  </si>
+  <si>
+    <t>Request Params longitudeSW, latitudeSW, longitudeNE and latitudeNE</t>
+  </si>
+  <si>
+    <t>Stories Count all of User by Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:8080/stories/count/user/screen?longitudeSW=45.78&amp;latitudeSW=4.8&amp;longitudeNE=45.8&amp;latitudeNE=5 </t>
+  </si>
+  <si>
+    <t>Count all stories of user given in header within the screen</t>
+  </si>
+  <si>
+    <t>Request Header "idUser" 
+Request Params longitudeSW, latitudeSW, longitudeNE and latitudeNE</t>
   </si>
 </sst>
 </file>
@@ -573,7 +598,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,9 +673,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -696,7 +718,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -715,7 +737,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -897,8 +919,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J1048571" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A1:J1048571">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J1048573" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A1:J1048573">
     <filterColumn colId="6"/>
   </autoFilter>
   <tableColumns count="10">
@@ -908,10 +930,10 @@
     <tableColumn id="4" name="Request type" dataDxfId="6"/>
     <tableColumn id="5" name="URL " dataDxfId="5"/>
     <tableColumn id="6" name="Test what ? " dataDxfId="4"/>
-    <tableColumn id="10" name="RequestHeader " dataDxfId="0"/>
-    <tableColumn id="7" name="Comments" dataDxfId="3"/>
-    <tableColumn id="8" name="Expected results" dataDxfId="2"/>
-    <tableColumn id="9" name="Results" dataDxfId="1"/>
+    <tableColumn id="10" name="RequestHeader " dataDxfId="3"/>
+    <tableColumn id="7" name="Comments" dataDxfId="2"/>
+    <tableColumn id="8" name="Expected results" dataDxfId="1"/>
+    <tableColumn id="9" name="Results" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1202,11 +1224,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1048571"/>
+  <dimension ref="A1:J1048573"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1367,7 +1389,7 @@
       <c r="I8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1397,11 +1419,11 @@
       <c r="I9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="13" customFormat="1">
+    <row r="10" spans="1:10" s="13" customFormat="1" ht="30">
       <c r="A10" s="22" t="s">
         <v>15</v>
       </c>
@@ -1409,27 +1431,29 @@
         <v>16</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="22"/>
+        <v>131</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>132</v>
+      </c>
       <c r="H10" s="24"/>
       <c r="I10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="13" customFormat="1">
+    <row r="11" spans="1:10" s="13" customFormat="1" ht="45">
       <c r="A11" s="22" t="s">
         <v>15</v>
       </c>
@@ -1437,29 +1461,29 @@
         <v>16</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="H11" s="24"/>
       <c r="I11" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="J11" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="13" customFormat="1" ht="30">
+    <row r="12" spans="1:10" s="13" customFormat="1">
       <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
@@ -1467,27 +1491,23 @@
         <v>16</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>128</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1499,27 +1519,29 @@
         <v>16</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="24"/>
+        <v>125</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="H13" s="24"/>
       <c r="I13" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="13" customFormat="1">
+    <row r="14" spans="1:10" s="13" customFormat="1" ht="30">
       <c r="A14" s="22" t="s">
         <v>15</v>
       </c>
@@ -1527,25 +1549,27 @@
         <v>16</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="24" t="s">
+        <v>128</v>
+      </c>
       <c r="I14" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1557,95 +1581,97 @@
         <v>16</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>123</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="13" customFormat="1">
+      <c r="A16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="13" customFormat="1">
+      <c r="A17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="22" t="s">
         <v>45</v>
-      </c>
-      <c r="J15" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="13" customFormat="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" s="13" customFormat="1">
-      <c r="A17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="14" t="s">
-        <v>23</v>
       </c>
       <c r="J17" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1">
-      <c r="A18" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" s="13" customFormat="1">
       <c r="A19" s="14" t="s">
@@ -1655,23 +1681,23 @@
         <v>49</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="15"/>
       <c r="I19" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1683,21 +1709,21 @@
         <v>49</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="15"/>
       <c r="I20" s="14" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="J20" s="19" t="s">
         <v>14</v>
@@ -1711,21 +1737,21 @@
         <v>49</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="15"/>
       <c r="I21" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>14</v>
@@ -1739,93 +1765,93 @@
         <v>49</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="15"/>
       <c r="I22" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J22" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="A23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1">
       <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24" s="14" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="J24" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="13" customFormat="1">
-      <c r="A25" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" s="13" customFormat="1">
       <c r="A26" s="14" t="s">
@@ -1835,23 +1861,23 @@
         <v>73</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="15"/>
       <c r="I26" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="J26" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1863,21 +1889,21 @@
         <v>73</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G27" s="14"/>
       <c r="H27" s="15"/>
       <c r="I27" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>14</v>
@@ -1891,21 +1917,21 @@
         <v>73</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="15"/>
       <c r="I28" s="14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J28" s="19" t="s">
         <v>14</v>
@@ -1919,93 +1945,93 @@
         <v>73</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G29" s="14"/>
       <c r="H29" s="15"/>
       <c r="I29" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J29" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="13" customFormat="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="A30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:10" s="13" customFormat="1">
       <c r="A31" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="15"/>
       <c r="I31" s="14" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="13" customFormat="1">
-      <c r="A32" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="J32" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" s="13" customFormat="1">
       <c r="A33" s="14" t="s">
@@ -2015,23 +2041,23 @@
         <v>97</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="15"/>
       <c r="I33" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="J33" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2043,21 +2069,21 @@
         <v>97</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="15"/>
       <c r="I34" s="14" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="J34" s="19" t="s">
         <v>14</v>
@@ -2071,21 +2097,21 @@
         <v>97</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="15"/>
       <c r="I35" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J35" s="19" t="s">
         <v>14</v>
@@ -2099,49 +2125,81 @@
         <v>97</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="15"/>
       <c r="I36" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J36" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="J36" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="13" customFormat="1">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
+      <c r="A37" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="G37" s="14"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
+      <c r="I37" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="1:10" s="13" customFormat="1">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="G38" s="14"/>
       <c r="H38" s="15"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
+      <c r="I38" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:10" s="13" customFormat="1">
       <c r="A39" s="14"/>
@@ -3259,52 +3317,78 @@
       <c r="I131" s="14"/>
       <c r="J131" s="14"/>
     </row>
-    <row r="1048571" spans="1:10">
-      <c r="A1048571" s="16"/>
-      <c r="B1048571" s="16"/>
-      <c r="C1048571" s="16"/>
-      <c r="D1048571" s="16"/>
-      <c r="E1048571" s="16"/>
-      <c r="F1048571" s="16"/>
-      <c r="G1048571" s="16"/>
-      <c r="H1048571" s="17"/>
-      <c r="I1048571" s="16"/>
-      <c r="J1048571" s="16"/>
+    <row r="132" spans="1:10" s="13" customFormat="1">
+      <c r="A132" s="14"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="14"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
+      <c r="F132" s="14"/>
+      <c r="G132" s="14"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="14"/>
+      <c r="J132" s="14"/>
+    </row>
+    <row r="133" spans="1:10" s="13" customFormat="1">
+      <c r="A133" s="14"/>
+      <c r="B133" s="14"/>
+      <c r="C133" s="14"/>
+      <c r="D133" s="14"/>
+      <c r="E133" s="14"/>
+      <c r="F133" s="14"/>
+      <c r="G133" s="14"/>
+      <c r="H133" s="15"/>
+      <c r="I133" s="14"/>
+      <c r="J133" s="14"/>
+    </row>
+    <row r="1048573" spans="1:10">
+      <c r="A1048573" s="16"/>
+      <c r="B1048573" s="16"/>
+      <c r="C1048573" s="16"/>
+      <c r="D1048573" s="16"/>
+      <c r="E1048573" s="16"/>
+      <c r="F1048573" s="16"/>
+      <c r="G1048573" s="16"/>
+      <c r="H1048573" s="17"/>
+      <c r="I1048573" s="16"/>
+      <c r="J1048573" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E10" r:id="rId1"/>
+    <hyperlink ref="E12" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
     <hyperlink ref="E8" r:id="rId3"/>
-    <hyperlink ref="E12" r:id="rId4"/>
-    <hyperlink ref="E13" r:id="rId5"/>
-    <hyperlink ref="E14" r:id="rId6"/>
-    <hyperlink ref="E15" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId4"/>
+    <hyperlink ref="E15" r:id="rId5"/>
+    <hyperlink ref="E16" r:id="rId6"/>
+    <hyperlink ref="E17" r:id="rId7"/>
     <hyperlink ref="E9" r:id="rId8"/>
-    <hyperlink ref="E11" r:id="rId9"/>
-    <hyperlink ref="E17" r:id="rId10"/>
-    <hyperlink ref="E18" r:id="rId11"/>
-    <hyperlink ref="E19" r:id="rId12"/>
-    <hyperlink ref="E20" r:id="rId13"/>
-    <hyperlink ref="E21" r:id="rId14"/>
-    <hyperlink ref="E22" r:id="rId15"/>
-    <hyperlink ref="E24" r:id="rId16"/>
-    <hyperlink ref="E25" r:id="rId17"/>
-    <hyperlink ref="E26" r:id="rId18"/>
-    <hyperlink ref="E27" r:id="rId19"/>
-    <hyperlink ref="E28" r:id="rId20"/>
-    <hyperlink ref="E29" r:id="rId21"/>
-    <hyperlink ref="E31" r:id="rId22"/>
-    <hyperlink ref="E32" r:id="rId23"/>
-    <hyperlink ref="E33" r:id="rId24"/>
-    <hyperlink ref="E34" r:id="rId25"/>
-    <hyperlink ref="E35" r:id="rId26"/>
-    <hyperlink ref="E36" r:id="rId27"/>
+    <hyperlink ref="E13" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+    <hyperlink ref="E20" r:id="rId11"/>
+    <hyperlink ref="E21" r:id="rId12"/>
+    <hyperlink ref="E22" r:id="rId13"/>
+    <hyperlink ref="E23" r:id="rId14"/>
+    <hyperlink ref="E24" r:id="rId15"/>
+    <hyperlink ref="E26" r:id="rId16"/>
+    <hyperlink ref="E27" r:id="rId17"/>
+    <hyperlink ref="E28" r:id="rId18"/>
+    <hyperlink ref="E29" r:id="rId19"/>
+    <hyperlink ref="E30" r:id="rId20"/>
+    <hyperlink ref="E31" r:id="rId21"/>
+    <hyperlink ref="E33" r:id="rId22"/>
+    <hyperlink ref="E34" r:id="rId23"/>
+    <hyperlink ref="E35" r:id="rId24"/>
+    <hyperlink ref="E36" r:id="rId25"/>
+    <hyperlink ref="E37" r:id="rId26"/>
+    <hyperlink ref="E38" r:id="rId27"/>
+    <hyperlink ref="E10" r:id="rId28"/>
+    <hyperlink ref="E11" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId29"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>